<commit_message>
fixing sheet_parser causing main, template not working
</commit_message>
<xml_diff>
--- a/tables_from_json_corrected.xlsx
+++ b/tables_from_json_corrected.xlsx
@@ -424,14 +424,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Report: MAM1.xlsx</t>
+          <t>Report Source: MAM1.xlsx</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sheet: 给徐燕打印</t>
+          <t>Worksheet: 给徐燕打印</t>
         </is>
       </c>
     </row>

</xml_diff>